<commit_message>
edit clickEvent(), edit save() +add saving tree
</commit_message>
<xml_diff>
--- a/excelhere/room_four.xlsx
+++ b/excelhere/room_four.xlsx
@@ -433,14 +433,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>442</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>